<commit_message>
Suporte para usuários do site antigo acessar o novo site sem trocar o password ;D
</commit_message>
<xml_diff>
--- a/server/Acessos INNBatível 2.0.xlsx
+++ b/server/Acessos INNBatível 2.0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Host</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Edit &gt; Settings ... Connection &gt; SFTP &gt; Add keyfile... Inserir o ssh/innb.ppk</t>
+  </si>
+  <si>
+    <t>cd .. &amp;&amp; cd .. &amp;&amp; cd cygdrive &amp;&amp; cd c &amp;&amp; cd Users &amp;&amp; cd w7innbativel &amp;&amp; cd Desktop &amp;&amp; ssh -i server/ssh/innb.pem ubuntu@54.209.79.205</t>
+  </si>
+  <si>
+    <t>cd .. &amp;&amp; cd .. &amp;&amp; cd var &amp;&amp; cd www</t>
   </si>
 </sst>
 </file>
@@ -585,7 +591,7 @@
   <dimension ref="B2:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -706,10 +712,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="4:4">
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
       <c r="D19" s="9"/>
     </row>
-    <row r="28" spans="4:4">
+    <row r="28" spans="2:4">
       <c r="D28" s="8"/>
     </row>
   </sheetData>

</xml_diff>